<commit_message>
Revisions to DFTO xls
Primary change - added sheet for ultramafic (copy/paste from OCFW - ultramafic savannah)

	modified:   DFTO Succession Transitions.xlsx
</commit_message>
<xml_diff>
--- a/_DFTO/DFTO Succession Transitions.xlsx
+++ b/_DFTO/DFTO Succession Transitions.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="0" windowWidth="18580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="12-7" sheetId="1" r:id="rId1"/>
+    <sheet name="DFTO 12-7" sheetId="1" r:id="rId1"/>
+    <sheet name="UM-0711700" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
   <si>
     <t>Succession Type</t>
   </si>
@@ -169,6 +170,18 @@
   </si>
   <si>
     <t>100% MC</t>
+  </si>
+  <si>
+    <t>Late Open 1</t>
+  </si>
+  <si>
+    <t>Late Open 2</t>
+  </si>
+  <si>
+    <t>100% go to MC</t>
+  </si>
+  <si>
+    <t>Probability of transition if mixed to:</t>
   </si>
 </sst>
 </file>
@@ -253,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,6 +278,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1846,4 +1860,1314 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="4"/>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10">
+        <v>200</v>
+      </c>
+      <c r="D2" s="7">
+        <v>200</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7">
+        <v>200</v>
+      </c>
+      <c r="G2" s="7">
+        <v>300</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="10"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="10"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
+        <v>15</v>
+      </c>
+      <c r="G6" s="10">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <f>1/C2</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D9" s="1">
+        <f>1/D2</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <f>1/F2</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="1">
+        <f>1/G2</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <f>C3</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1">
+        <f>C10</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <f>D10</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <f>F10</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f>G10</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="S12" s="6"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <f>1/C6</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <f>1/D6</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <f>1/F6</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <f>1/G6</f>
+        <v>0.05</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <f>C9+C13</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <f>D9</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <f>F9+F11</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G14" s="1">
+        <f>G9+G11</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="H14" s="1">
+        <f>SUM(C14:G14)</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <f>D13</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <f>F12+F13</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <f>G12+G13</f>
+        <v>0.05</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(C15:G15)</f>
+        <v>0.18333333333333335</v>
+      </c>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="J16" s="6"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1">
+        <f>C9+C10+C13</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <f>D9+D10+D13</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <f>F9+F10+F13</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <f>G9+G10+G13</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="H17" s="1">
+        <f>SUM(C17:G17)</f>
+        <v>0.26833333333333337</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="S17" s="6"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <f>C14+C15</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <f>D14+D15</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <f>F14+F15</f>
+        <v>7.166666666666667E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <f>G14+G15</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="6">
+        <f>(D10+D13/2)/D15</f>
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <f>F10/F15</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>G10/G15</f>
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <f>(D13/2)/D15</f>
+        <v>0.5</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>5</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <f>G24/G15</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f>J24/G31</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="R24" s="6"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <f>F13/F15</f>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f>G13/G15</f>
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <f>G25/G15</f>
+        <v>20</v>
+      </c>
+      <c r="K25" s="1">
+        <f>J25/G31</f>
+        <v>21.333333333333332</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="J28" s="6"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <f>C17/$H$17</f>
+        <v>0.26708074534161491</v>
+      </c>
+      <c r="D29">
+        <f>D17/$H$17</f>
+        <v>0.26708074534161491</v>
+      </c>
+      <c r="F29">
+        <f>F17/$H$17</f>
+        <v>0.26708074534161491</v>
+      </c>
+      <c r="G29">
+        <f>G17/$H$17</f>
+        <v>0.19875776397515527</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <f>C14/C17</f>
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f>D14/D17</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="F30">
+        <f>F14/F17</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="G30">
+        <f>G14/G17</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31">
+        <f>C15/C17</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f>D15/D17</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="F31">
+        <f>F15/F17</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="G31">
+        <f>G15/G17</f>
+        <v>0.9375</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="7"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="7"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <f>C30+C31</f>
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <f>D14/D17</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="F34">
+        <f>F9/F17</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+      <c r="G34">
+        <f>G9/G17</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <f>F10/F17</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f>G10/G17</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <f>D31</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="H36">
+        <f>H17/$H$17</f>
+        <v>1</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <f>F13/F17</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="H37">
+        <f>H14/$H$14</f>
+        <v>1</v>
+      </c>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38">
+        <f>G13/G17</f>
+        <v>0.9375</v>
+      </c>
+      <c r="H38">
+        <f>H15/$H$15</f>
+        <v>1</v>
+      </c>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39">
+        <f>SUM(C34:C38)</f>
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <f>SUM(D34:D38)</f>
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <f>SUM(F34:F37)</f>
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <f>SUM(G34:G38)</f>
+        <v>1</v>
+      </c>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <v>0.1</v>
+      </c>
+      <c r="D42">
+        <v>0.3</v>
+      </c>
+      <c r="F42">
+        <v>0.5</v>
+      </c>
+      <c r="G42">
+        <v>0.1</v>
+      </c>
+      <c r="H42">
+        <f>SUM(C42:G42)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <f>C17*C42</f>
+        <v>7.1666666666666675E-3</v>
+      </c>
+      <c r="D44">
+        <f>D17*D42</f>
+        <v>2.1500000000000002E-2</v>
+      </c>
+      <c r="F44">
+        <f>F17*F42</f>
+        <v>3.5833333333333335E-2</v>
+      </c>
+      <c r="G44">
+        <f>G17*G42</f>
+        <v>5.333333333333334E-3</v>
+      </c>
+      <c r="H44">
+        <f>SUM(C44:G44)</f>
+        <v>6.9833333333333331E-2</v>
+      </c>
+      <c r="Q44" s="7"/>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <f>C14*C42</f>
+        <v>7.1666666666666675E-3</v>
+      </c>
+      <c r="D45">
+        <f>D14*D42</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="F45">
+        <f>F14*F42</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G45">
+        <f>G14*G42</f>
+        <v>3.3333333333333338E-4</v>
+      </c>
+      <c r="H45">
+        <f>SUM(C45:G45)</f>
+        <v>1.1500000000000002E-2</v>
+      </c>
+      <c r="Q45" s="7"/>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <f>C15*C42</f>
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <f>D15*D42</f>
+        <v>0.02</v>
+      </c>
+      <c r="F46">
+        <f>F15*F42</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G46">
+        <f>G15*G42</f>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="H46">
+        <f>SUM(C46:G46)</f>
+        <v>5.8333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" t="s">
+        <v>36</v>
+      </c>
+      <c r="J49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="1">
+        <f>1/C50</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="C50">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D50">
+        <f>C50/C55</f>
+        <v>2.2656899025753342E-2</v>
+      </c>
+      <c r="F50">
+        <f>F55*D50</f>
+        <v>1.5822067819651084E-3</v>
+      </c>
+      <c r="H50">
+        <f>H45</f>
+        <v>1.1500000000000002E-2</v>
+      </c>
+      <c r="I50">
+        <f>1/H50</f>
+        <v>86.956521739130423</v>
+      </c>
+      <c r="J50">
+        <f>H50/H55*100</f>
+        <v>16.467780429594274</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="1">
+        <f>1/C51</f>
+        <v>34.002040122407344</v>
+      </c>
+      <c r="C51">
+        <v>2.9409999999999999E-2</v>
+      </c>
+      <c r="D51">
+        <f>C51/C55</f>
+        <v>0.22211313344913525</v>
+      </c>
+      <c r="F51">
+        <f>F55*D51</f>
+        <v>1.551090048586461E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="1">
+        <f>1/C54</f>
+        <v>10</v>
+      </c>
+      <c r="C54">
+        <v>0.1</v>
+      </c>
+      <c r="D54">
+        <f>C54/C55</f>
+        <v>0.7552299675251114</v>
+      </c>
+      <c r="F54">
+        <f>F55*D54</f>
+        <v>5.2740226065503611E-2</v>
+      </c>
+      <c r="H54">
+        <f>H46</f>
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="I54">
+        <f>1/H54</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="J54">
+        <f>H54/H55*100</f>
+        <v>83.532219570405729</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="1">
+        <f>1/C55</f>
+        <v>7.5522996752511142</v>
+      </c>
+      <c r="C55">
+        <v>0.13241</v>
+      </c>
+      <c r="D55">
+        <f>D50+D51+D54</f>
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <f>H44</f>
+        <v>6.9833333333333331E-2</v>
+      </c>
+      <c r="H55">
+        <f>H50+H54</f>
+        <v>6.9833333333333331E-2</v>
+      </c>
+      <c r="I55">
+        <f>1/H55</f>
+        <v>14.319809069212411</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="J62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+    </row>
+    <row r="75" spans="2:8">
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+    </row>
+    <row r="77" spans="2:8">
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update DFTO Succession Transitions
Includes ultramafic tab. May only be small changes to format.

	modified:   _DFTO/DFTO Succession Transitions.xlsx
</commit_message>
<xml_diff>
--- a/_DFTO/DFTO Succession Transitions.xlsx
+++ b/_DFTO/DFTO Succession Transitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="21940" windowHeight="19960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DFTO 12-7" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +204,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,8 +279,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -280,7 +298,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1854,6 +1874,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1866,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>

</xml_diff>